<commit_message>
Running bipolar moto with PWM signal
- integration of the PWM (Output compare module) in the FW
- Running bipolar motor with PWM / DIR inputs
</commit_message>
<xml_diff>
--- a/Documentation/FW_Information.xlsx
+++ b/Documentation/FW_Information.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Use of timers</t>
   </si>
@@ -402,7 +402,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,6 +448,9 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Start to work on the STEST command
</commit_message>
<xml_diff>
--- a/Documentation/FW_Information.xlsx
+++ b/Documentation/FW_Information.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TIMERS" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Use of timers</t>
   </si>
@@ -140,6 +143,9 @@
   </si>
   <si>
     <t>HW version</t>
+  </si>
+  <si>
+    <t>Test byte for STEST command (will be read, incremented, write and read once again to test R/W functions)</t>
   </si>
 </sst>
 </file>
@@ -259,7 +265,35 @@
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="14">
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="&quot;0x&quot;##"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -320,94 +354,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;0x&quot;##"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -431,7 +377,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A5:F260" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A5:F260" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A5:F260">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -441,16 +387,16 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Address" dataDxfId="14"/>
-    <tableColumn id="2" name="Address hex" dataDxfId="13">
+    <tableColumn id="1" name="Address" dataDxfId="5"/>
+    <tableColumn id="2" name="Address hex" dataDxfId="4">
       <calculatedColumnFormula>DEC2HEX(A6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Access (user)" dataDxfId="12"/>
-    <tableColumn id="4" name="Default value" dataDxfId="11"/>
-    <tableColumn id="6" name="Default value hex" dataDxfId="10">
+    <tableColumn id="3" name="Access (user)" dataDxfId="3"/>
+    <tableColumn id="4" name="Default value" dataDxfId="2"/>
+    <tableColumn id="6" name="Default value hex" dataDxfId="1">
       <calculatedColumnFormula>IF(Tableau2[[#This Row],[Default value]]&lt;&gt;"",CONCATENATE("0x",DEC2HEX(Tableau2[[#This Row],[Default value]],2)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Description" dataDxfId="9"/>
+    <tableColumn id="5" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,7 +770,7 @@
   <dimension ref="A1:F260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,10 +1152,18 @@
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
       <c r="E21" s="4" t="str">
         <f>IF(Tableau2[[#This Row],[Default value]]&lt;&gt;"",CONCATENATE("0x",DEC2HEX(Tableau2[[#This Row],[Default value]],2)),"")</f>
-        <v/>
+        <v>0x00</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -4563,24 +4517,24 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:C18 C21:C260">
-    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="NO ACCESS">
+    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="NO ACCESS">
       <formula>NOT(ISERROR(SEARCH("NO ACCESS",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="5" operator="containsText" text="READ ONLY">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="READ ONLY">
       <formula>NOT(ISERROR(SEARCH("READ ONLY",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="READ/WRITE">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="READ/WRITE">
       <formula>NOT(ISERROR(SEARCH("READ/WRITE",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="READ/WRITE">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="READ/WRITE">
       <formula>NOT(ISERROR(SEARCH("READ/WRITE",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="READ ONLY">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="READ ONLY">
       <formula>NOT(ISERROR(SEARCH("READ ONLY",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="NO ACCESS">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="NO ACCESS">
       <formula>NOT(ISERROR(SEARCH("NO ACCESS",C19)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>